<commit_message>
fix counting and calculation errors
</commit_message>
<xml_diff>
--- a/data/translate/output/translate_misspellings_1000.xlsx
+++ b/data/translate/output/translate_misspellings_1000.xlsx
@@ -3717,11 +3717,11 @@
   </sheetPr>
   <dimension ref="A1:F1020"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1000" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1011" activeCellId="0" sqref="B1011"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A999" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1009" activeCellId="0" sqref="A1009:B1014"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.72"/>
@@ -10131,6 +10131,12 @@
         <v>75</v>
       </c>
     </row>
+    <row r="1011" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1011" s="3"/>
+    </row>
+    <row r="1013" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1013" s="3"/>
+    </row>
     <row r="1015" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1015" s="3"/>
     </row>

</xml_diff>